<commit_message>
Modify Application Interface:   - Add second screen;   - Add interaction;
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -141,6 +141,21 @@
   </si>
   <si>
     <t xml:space="preserve">Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ILI9341 240x320</t>
   </si>
 </sst>
 </file>
@@ -1601,6 +1616,23 @@
         <v>36</v>
       </c>
     </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>